<commit_message>
[EDIT] error buildings import
</commit_message>
<xml_diff>
--- a/test_many_import.xlsx
+++ b/test_many_import.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frogman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frogman/Documents/INSECTO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F1BF7A-1726-E44B-B897-48C1CA14A6FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA515B20-D2A3-664F-B00C-433F5822F80D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Buildings" sheetId="3" r:id="rId1"/>
+    <sheet name="Buildings" sheetId="7" r:id="rId1"/>
     <sheet name="Rooms" sheetId="1" r:id="rId2"/>
     <sheet name="Item_Types" sheetId="4" r:id="rId3"/>
     <sheet name="Problem_Descriptions" sheetId="6" r:id="rId4"/>
@@ -115,38 +115,38 @@
     <t>TEST-10</t>
   </si>
   <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>type_name</t>
+  </si>
+  <si>
+    <t>brand_name</t>
+  </si>
+  <si>
+    <t>problem_description</t>
+  </si>
+  <si>
     <t>building_code</t>
   </si>
   <si>
     <t>building_name</t>
   </si>
   <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>World</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>world</t>
-  </si>
-  <si>
-    <t>type_name</t>
-  </si>
-  <si>
-    <t>brand_name</t>
-  </si>
-  <si>
-    <t>problem_description</t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>kub</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,12 +172,6 @@
     <font>
       <sz val="24"/>
       <color theme="1"/>
-      <name val="TH SarabunPSK"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
       <name val="TH SarabunPSK"/>
       <family val="2"/>
     </font>
@@ -209,25 +203,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,171 +532,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0856EA2C-A850-B34A-8F08-87498E462308}">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0DCBAA-EC39-644D-94F0-CFE52484AEA9}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="36" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="19.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -717,67 +599,67 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="36" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2">
         <v>1</v>
       </c>
     </row>
@@ -798,74 +680,74 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="36" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="2" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="2" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
         <v>1</v>
       </c>
     </row>
@@ -885,164 +767,164 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="36" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5">
-        <v>2</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5">
-        <v>2</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="5">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="5">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="B11" s="2">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1062,97 +944,97 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="36" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1166,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1186,307 +1068,307 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="36" x14ac:dyDescent="0.6">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="5">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
-        <v>2</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="5">
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.6">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="5">
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="36" x14ac:dyDescent="0.6">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <v>2</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="5">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="36" x14ac:dyDescent="0.6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>2</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="5">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="36" x14ac:dyDescent="0.6">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
-        <v>2</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" s="5">
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="36" x14ac:dyDescent="0.6">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>2</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="5">
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="36" x14ac:dyDescent="0.6">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5">
-        <v>2</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K9" s="5">
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="36" x14ac:dyDescent="0.6">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K10" s="5">
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="36" x14ac:dyDescent="0.6">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5">
-        <v>2</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="5">
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>